<commit_message>
Disable test for formula with tags; fix template for not using formulas with tags inside
Upgrading to ClosedXML 0.100 broke this functionality: previously it was possible to put a formula inside a cell and then to retrieve an original value it had (e.g. &="Total:"<<sum>>). Now this does not work (which is correct) and making it right would require somewhat major refactoring for which no one has time
</commit_message>
<xml_diff>
--- a/tests/Templates/GroupTagTests_TotalLabel.xlsx
+++ b/tests/Templates/GroupTagTests_TotalLabel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20400"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\opensource\ClosedXML.Report\tests\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F730A8D9-6D61-4C44-A11D-F3EE9BFD5E7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="615" windowWidth="15480" windowHeight="11460"/>
+    <workbookView xWindow="600" yWindow="612" windowWidth="15480" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,19 +82,19 @@
     <t>Company</t>
   </si>
   <si>
-    <t>&amp;="Total: "&lt;&lt;sum&gt;&gt;</t>
-  </si>
-  <si>
     <t>&lt;&lt;group TotalLabel="Company Total: "  GrandLabel="Grand: "&gt;&gt;</t>
   </si>
   <si>
     <t>&lt;&lt;group mergelabels=merge2  TotalLabel=""&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;sum&gt;&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
@@ -314,7 +320,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -390,6 +396,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -411,7 +420,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2" descr="logo.png"/>
+        <xdr:cNvPr id="3" name="Рисунок 2" descr="logo.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -784,7 +799,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -792,19 +807,19 @@
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="11" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="11" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="19" t="s">
         <v>7</v>
@@ -817,7 +832,7 @@
       <c r="H1" s="18"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -841,7 +856,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="7" t="s">
         <v>17</v>
@@ -900,16 +915,16 @@
         <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="10"/>
       <c r="G6" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="15"/>

</xml_diff>

<commit_message>
Bump closedxml to v.0.100.3 (#307)
* Updated dependencies
* Bump to ClosedXML 0.100.3
* Fix assigning formulas in group totals
* Disable test for formula with tags; fix template for not using formulas with tags inside

Upgrading to ClosedXML 0.100 broke this functionality: previously it was possible to put a formula inside a cell and then to retrieve an original value it had (e.g. &="Total:"<<sum>>). Now this does not work (which is correct) and making it right would require somewhat major refactoring for which no one has time

Co-authored-by: Aleksei <pankraty@gmail.com>
</commit_message>
<xml_diff>
--- a/tests/Templates/GroupTagTests_TotalLabel.xlsx
+++ b/tests/Templates/GroupTagTests_TotalLabel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20400"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\opensource\ClosedXML.Report\tests\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F730A8D9-6D61-4C44-A11D-F3EE9BFD5E7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="615" windowWidth="15480" windowHeight="11460"/>
+    <workbookView xWindow="600" yWindow="612" windowWidth="15480" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,19 +82,19 @@
     <t>Company</t>
   </si>
   <si>
-    <t>&amp;="Total: "&lt;&lt;sum&gt;&gt;</t>
-  </si>
-  <si>
     <t>&lt;&lt;group TotalLabel="Company Total: "  GrandLabel="Grand: "&gt;&gt;</t>
   </si>
   <si>
     <t>&lt;&lt;group mergelabels=merge2  TotalLabel=""&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;sum&gt;&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
@@ -314,7 +320,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -390,6 +396,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -411,7 +420,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2" descr="logo.png"/>
+        <xdr:cNvPr id="3" name="Рисунок 2" descr="logo.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -784,7 +799,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -792,19 +807,19 @@
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="11" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="11" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="19" t="s">
         <v>7</v>
@@ -817,7 +832,7 @@
       <c r="H1" s="18"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -841,7 +856,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="7" t="s">
         <v>17</v>
@@ -900,16 +915,16 @@
         <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="10"/>
       <c r="G6" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="15"/>

</xml_diff>